<commit_message>
Default pre-allocated blocks for HIGH_PERF raised, (Debug) Display of internal data sizes memory sheet updated for V2
git-svn-id: https://svn.code.sf.net/p/tcnopen/trdp/trunk@2005 3b5a3598-5f4e-4449-9e63-bd40438bfec0
</commit_message>
<xml_diff>
--- a/trdp/doc/memory.xlsx
+++ b/trdp/doc/memory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bloehr/Repos-Projekte/tcnopen-trdp/trunk/trdp/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18BF16CA-72CB-9741-8457-5B811E193202}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84C8E85-1DFE-044F-BAAE-D900A91DE2C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="960" windowWidth="26500" windowHeight="19100" tabRatio="500"/>
+    <workbookView xWindow="-29580" yWindow="1060" windowWidth="26500" windowHeight="19100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,13 @@
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>Memory consumption (all values in Bytes):</t>
   </si>
@@ -132,14 +132,23 @@
     <t>128 + n</t>
   </si>
   <si>
-    <t>(needs update for V2)</t>
+    <t>MD_SUPPORT == 1 + HIGH_PERF_INDEXED</t>
+  </si>
+  <si>
+    <t>will be allocated in 3 arrays</t>
+  </si>
+  <si>
+    <t>will be allocated in 2 arrays</t>
+  </si>
+  <si>
+    <t>(Updated for V2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +169,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -189,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -209,6 +226,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -295,9 +313,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Bernd Löhr" refreshedDate="41389.577807870373" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="104">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Bernd Löhr" refreshedDate="41389.577807870373" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="104" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B16:B124" sheet="Blatt1"/>
+    <worksheetSource ref="B16:B126" sheet="Blatt1"/>
   </cacheSource>
   <cacheFields count="1">
     <cacheField name="296" numFmtId="0">
@@ -317,7 +335,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:F16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField showAll="0"/>
@@ -652,8 +670,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -678,7 +696,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1180,21 +1198,340 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="4"/>
+      <c r="A52" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G53" s="4"/>
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="2">
+        <v>48</v>
+      </c>
+      <c r="F53" s="2">
+        <v>48</v>
+      </c>
+      <c r="G53" s="4">
+        <f>F53</f>
+        <v>48</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2">
+        <v>14200</v>
+      </c>
+      <c r="F54" s="2">
+        <v>16384</v>
+      </c>
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E55" s="2">
+        <v>48</v>
+      </c>
+      <c r="F55" s="2">
+        <v>48</v>
+      </c>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E56" s="2">
+        <v>128</v>
+      </c>
+      <c r="F56" s="8">
+        <v>128</v>
+      </c>
       <c r="G56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E57" s="2">
+        <v>416</v>
+      </c>
+      <c r="F57" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E58" s="8">
+        <v>128</v>
+      </c>
+      <c r="F58" s="8">
+        <v>128</v>
+      </c>
+      <c r="G58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E59" s="8">
+        <v>1472</v>
+      </c>
+      <c r="F59" s="8">
+        <v>1480</v>
+      </c>
+      <c r="G59" s="4">
+        <f>SUM(F54:F59)</f>
+        <v>18680</v>
+      </c>
+      <c r="H59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="2">
+        <v>128</v>
+      </c>
+      <c r="F61" s="8">
+        <v>128</v>
+      </c>
+      <c r="G61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E62" s="2">
+        <v>16</v>
+      </c>
+      <c r="F62" s="8">
+        <v>16</v>
+      </c>
+      <c r="G62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E63" s="2">
+        <v>1472</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1480</v>
+      </c>
+      <c r="G63" s="4">
+        <f>SUM(F61:F63)</f>
+        <v>1624</v>
+      </c>
+      <c r="H63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="2">
+        <v>128</v>
+      </c>
+      <c r="F66" s="8">
+        <v>128</v>
+      </c>
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E67" s="2">
+        <v>72</v>
+      </c>
+      <c r="F67" s="2">
+        <v>72</v>
+      </c>
+      <c r="G67" s="4"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" s="2">
+        <v>180</v>
+      </c>
+      <c r="F68" s="2">
+        <v>180</v>
+      </c>
+      <c r="G68" s="4"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E69" s="2">
+        <v>1472</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1480</v>
+      </c>
+      <c r="G69" s="4">
+        <f>SUM(F66:F69)</f>
+        <v>1860</v>
+      </c>
+      <c r="H69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="2">
+        <v>212</v>
+      </c>
+      <c r="F71" s="2">
+        <v>256</v>
+      </c>
+      <c r="G71" s="4"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="4"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>25</v>
+      </c>
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="4"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78" s="2">
+        <v>84</v>
+      </c>
+      <c r="F78" s="2">
+        <v>84</v>
+      </c>
+      <c r="G78" s="4">
+        <f>F78</f>
+        <v>84</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>31</v>
+      </c>
+      <c r="E80" s="2">
+        <v>212</v>
+      </c>
+      <c r="F80" s="2">
+        <v>256</v>
+      </c>
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E81" s="2">
+        <v>1480</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1480</v>
+      </c>
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>30</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="4">
+        <f>SUM(F80:F82)</f>
+        <v>1736</v>
+      </c>
+      <c r="H82" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
@@ -1204,7 +1541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>